<commit_message>
Last commit part 1 - After creating the dataset_covid_10_countries before visualisation
</commit_message>
<xml_diff>
--- a/team9/files/Datasets/dataset_final_WGI_capacity_access.xlsx
+++ b/team9/files/Datasets/dataset_final_WGI_capacity_access.xlsx
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="C8">
-        <v>53230</v>
+        <v>53250</v>
       </c>
       <c r="D8">
         <v>83.98</v>
@@ -673,7 +673,7 @@
         </is>
       </c>
       <c r="C9">
-        <v>49310</v>
+        <v>49350</v>
       </c>
       <c r="D9">
         <v>86.53</v>
@@ -781,7 +781,7 @@
         </is>
       </c>
       <c r="C12">
-        <v>45910</v>
+        <v>45870</v>
       </c>
       <c r="D12">
         <v>87.25</v>
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="C13">
-        <v>870</v>
+        <v>1200</v>
       </c>
       <c r="D13">
         <v>69.68000000000001</v>
@@ -1033,7 +1033,7 @@
         </is>
       </c>
       <c r="C19">
-        <v>5670</v>
+        <v>5700</v>
       </c>
       <c r="D19">
         <v>47.57</v>
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="C21">
-        <v>9140</v>
+        <v>9080</v>
       </c>
       <c r="D21">
         <v>66.42</v>
@@ -1249,7 +1249,7 @@
         </is>
       </c>
       <c r="C25">
-        <v>44940</v>
+        <v>44950</v>
       </c>
       <c r="D25">
         <v>83.47</v>
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="C26">
-        <v>84410</v>
+        <v>84450</v>
       </c>
       <c r="D26">
         <v>87.87</v>
@@ -1681,7 +1681,7 @@
         </is>
       </c>
       <c r="C37">
-        <v>20240</v>
+        <v>20230</v>
       </c>
       <c r="D37">
         <v>83.09</v>
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="C38">
-        <v>47090</v>
+        <v>47110</v>
       </c>
       <c r="D38">
         <v>85.03</v>
@@ -1789,7 +1789,7 @@
         </is>
       </c>
       <c r="C40">
-        <v>60140</v>
+        <v>60170</v>
       </c>
       <c r="D40">
         <v>89.64</v>
@@ -1933,7 +1933,7 @@
         </is>
       </c>
       <c r="C44">
-        <v>29340</v>
+        <v>29300</v>
       </c>
       <c r="D44">
         <v>81.31</v>
@@ -1969,7 +1969,7 @@
         </is>
       </c>
       <c r="C45">
-        <v>21140</v>
+        <v>21130</v>
       </c>
       <c r="D45">
         <v>86.45</v>
@@ -2041,7 +2041,7 @@
         </is>
       </c>
       <c r="C47">
-        <v>48280</v>
+        <v>48300</v>
       </c>
       <c r="D47">
         <v>91.08</v>
@@ -2077,7 +2077,7 @@
         </is>
       </c>
       <c r="C48">
-        <v>41080</v>
+        <v>41090</v>
       </c>
       <c r="D48">
         <v>77.76000000000001</v>
@@ -2149,7 +2149,7 @@
         </is>
       </c>
       <c r="C50">
-        <v>41770</v>
+        <v>41790</v>
       </c>
       <c r="D50">
         <v>77.73999999999999</v>
@@ -2185,7 +2185,7 @@
         </is>
       </c>
       <c r="C51">
-        <v>4440</v>
+        <v>4450</v>
       </c>
       <c r="D51">
         <v>72.23999999999999</v>
@@ -2365,7 +2365,7 @@
         </is>
       </c>
       <c r="C56">
-        <v>6840</v>
+        <v>6650</v>
       </c>
       <c r="D56">
         <v>33.53</v>
@@ -2401,7 +2401,7 @@
         </is>
       </c>
       <c r="C57">
-        <v>19770</v>
+        <v>19760</v>
       </c>
       <c r="D57">
         <v>69.11</v>
@@ -2509,7 +2509,7 @@
         </is>
       </c>
       <c r="C60">
-        <v>2350</v>
+        <v>2320</v>
       </c>
       <c r="D60">
         <v>56.25</v>
@@ -2617,7 +2617,7 @@
         </is>
       </c>
       <c r="C63">
-        <v>14780</v>
+        <v>14760</v>
       </c>
       <c r="D63">
         <v>70.98999999999999</v>
@@ -2725,7 +2725,7 @@
         </is>
       </c>
       <c r="C66">
-        <v>61390</v>
+        <v>61210</v>
       </c>
       <c r="D66">
         <v>85.92</v>
@@ -2797,7 +2797,7 @@
         </is>
       </c>
       <c r="C68">
-        <v>67960</v>
+        <v>68120</v>
       </c>
       <c r="D68">
         <v>86.97</v>
@@ -2833,7 +2833,7 @@
         </is>
       </c>
       <c r="C69">
-        <v>40920</v>
+        <v>40930</v>
       </c>
       <c r="D69">
         <v>68.98999999999999</v>
@@ -2869,7 +2869,7 @@
         </is>
       </c>
       <c r="C70">
-        <v>33730</v>
+        <v>33740</v>
       </c>
       <c r="D70">
         <v>73.73999999999999</v>
@@ -3013,7 +3013,7 @@
         </is>
       </c>
       <c r="C74">
-        <v>8070</v>
+        <v>8080</v>
       </c>
       <c r="D74">
         <v>45.99</v>
@@ -3157,7 +3157,7 @@
         </is>
       </c>
       <c r="C78">
-        <v>30600</v>
+        <v>30620</v>
       </c>
       <c r="D78">
         <v>72.39</v>
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="C86">
-        <v>17430</v>
+        <v>17360</v>
       </c>
       <c r="D86">
         <v>78.63</v>
@@ -3481,7 +3481,7 @@
         </is>
       </c>
       <c r="C87">
-        <v>70870</v>
+        <v>70840</v>
       </c>
       <c r="D87">
         <v>85.28</v>
@@ -3517,7 +3517,7 @@
         </is>
       </c>
       <c r="C88">
-        <v>16510</v>
+        <v>16500</v>
       </c>
       <c r="D88">
         <v>81.38</v>
@@ -3589,7 +3589,7 @@
         </is>
       </c>
       <c r="C90">
-        <v>2980</v>
+        <v>3900</v>
       </c>
       <c r="D90">
         <v>69.59</v>
@@ -4129,7 +4129,7 @@
         </is>
       </c>
       <c r="C105">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="D105">
         <v>68.98999999999999</v>
@@ -4201,7 +4201,7 @@
         </is>
       </c>
       <c r="C107">
-        <v>80610</v>
+        <v>80640</v>
       </c>
       <c r="D107">
         <v>92.40000000000001</v>
@@ -4273,7 +4273,7 @@
         </is>
       </c>
       <c r="C109">
-        <v>40640</v>
+        <v>41020</v>
       </c>
       <c r="D109">
         <v>86.02</v>
@@ -4561,7 +4561,7 @@
         </is>
       </c>
       <c r="C117">
-        <v>21990</v>
+        <v>21980</v>
       </c>
       <c r="D117">
         <v>84.23</v>
@@ -5029,7 +5029,7 @@
         </is>
       </c>
       <c r="C130">
-        <v>24580</v>
+        <v>24500</v>
       </c>
       <c r="D130">
         <v>78.3</v>
@@ -5065,7 +5065,7 @@
         </is>
       </c>
       <c r="C131">
-        <v>55490</v>
+        <v>55540</v>
       </c>
       <c r="D131">
         <v>91.73</v>
@@ -5533,7 +5533,7 @@
         </is>
       </c>
       <c r="C144">
-        <v>63080</v>
+        <v>63170</v>
       </c>
       <c r="D144">
         <v>76.12</v>

</xml_diff>